<commit_message>
update gumbel according to the slides
</commit_message>
<xml_diff>
--- a/devoir2_results.xlsx
+++ b/devoir2_results.xlsx
@@ -500,13 +500,13 @@
         <v>0.3682487299061701</v>
       </c>
       <c r="F2" t="n">
-        <v>4.680675833021207</v>
+        <v>4.680675833021208</v>
       </c>
       <c r="G2" t="n">
         <v>35.61873608701515</v>
       </c>
       <c r="H2" t="n">
-        <v>115.4431759978146</v>
+        <v>115.443181612837</v>
       </c>
     </row>
     <row r="3">
@@ -534,7 +534,7 @@
         <v>41.59439954231561</v>
       </c>
       <c r="H3" t="n">
-        <v>119.2151231318074</v>
+        <v>119.215127940147</v>
       </c>
     </row>
     <row r="4">
@@ -553,7 +553,7 @@
         <v>4.702642173211798</v>
       </c>
       <c r="E4" t="n">
-        <v>0.3516687104736785</v>
+        <v>0.3516687104736786</v>
       </c>
       <c r="F4" t="n">
         <v>4.706324657274862</v>
@@ -562,7 +562,7 @@
         <v>35.18465307571481</v>
       </c>
       <c r="H4" t="n">
-        <v>117.8455951203282</v>
+        <v>117.8456008046247</v>
       </c>
     </row>
   </sheetData>
@@ -639,10 +639,10 @@
         <v>0.008936958889347892</v>
       </c>
       <c r="C2" t="n">
-        <v>0.007487614647643717</v>
+        <v>0.007487614647643662</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0005950610170728506</v>
+        <v>0.0005950603203842252</v>
       </c>
       <c r="E2" t="n">
         <v>0.0119047619047619</v>
@@ -654,10 +654,10 @@
         <v>0.01487256492017592</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01632190916188009</v>
+        <v>0.01632190916188015</v>
       </c>
       <c r="I2" t="n">
-        <v>0.02321446279245096</v>
+        <v>0.02321446348913958</v>
       </c>
     </row>
     <row r="3">
@@ -668,10 +668,10 @@
         <v>0.06250023432670739</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05719022568203853</v>
+        <v>0.05719022568203825</v>
       </c>
       <c r="D3" t="n">
-        <v>0.009066562770240941</v>
+        <v>0.009066556048133119</v>
       </c>
       <c r="E3" t="n">
         <v>0.03571428571428571</v>
@@ -683,10 +683,10 @@
         <v>0.01488118670765977</v>
       </c>
       <c r="H3" t="n">
-        <v>0.009571178062990911</v>
+        <v>0.009571178062990633</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03855248484880668</v>
+        <v>0.0385524915709145</v>
       </c>
     </row>
     <row r="4">
@@ -697,10 +697,10 @@
         <v>0.1431643623253325</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1357446988910646</v>
+        <v>0.135744698891064</v>
       </c>
       <c r="D4" t="n">
-        <v>0.03362611369742202</v>
+        <v>0.03362609571437278</v>
       </c>
       <c r="E4" t="n">
         <v>0.05952380952380952</v>
@@ -712,10 +712,10 @@
         <v>0.0717357908967611</v>
       </c>
       <c r="H4" t="n">
-        <v>0.06431612746249313</v>
+        <v>0.06431612746249257</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0378024577311494</v>
+        <v>0.03780247571419864</v>
       </c>
     </row>
     <row r="5">
@@ -726,10 +726,10 @@
         <v>0.1523767148425946</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1448541431831825</v>
+        <v>0.144854143183182</v>
       </c>
       <c r="D5" t="n">
-        <v>0.03724949282019956</v>
+        <v>0.03724947350031146</v>
       </c>
       <c r="E5" t="n">
         <v>0.08333333333333333</v>
@@ -741,10 +741,10 @@
         <v>0.0571386196044994</v>
       </c>
       <c r="H5" t="n">
-        <v>0.04961604794508728</v>
+        <v>0.04961604794508673</v>
       </c>
       <c r="I5" t="n">
-        <v>0.05798860241789567</v>
+        <v>0.05798862173778377</v>
       </c>
     </row>
     <row r="6">
@@ -755,10 +755,10 @@
         <v>0.1623293156293571</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1547187596300525</v>
+        <v>0.1547187596300518</v>
       </c>
       <c r="D6" t="n">
-        <v>0.04134654635219388</v>
+        <v>0.04134652558747407</v>
       </c>
       <c r="E6" t="n">
         <v>0.1071428571428571</v>
@@ -770,10 +770,10 @@
         <v>0.04328169658173806</v>
       </c>
       <c r="H6" t="n">
-        <v>0.03567114058243345</v>
+        <v>0.03567114058243279</v>
       </c>
       <c r="I6" t="n">
-        <v>0.07770107269542517</v>
+        <v>0.07770109346014498</v>
       </c>
     </row>
     <row r="7">
@@ -784,10 +784,10 @@
         <v>0.1651047922720605</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1574737636531398</v>
+        <v>0.1574737636531391</v>
       </c>
       <c r="D7" t="n">
-        <v>0.04252271984475932</v>
+        <v>0.04252269867737873</v>
       </c>
       <c r="E7" t="n">
         <v>0.130952380952381</v>
@@ -799,10 +799,10 @@
         <v>0.02224764941491769</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0146166207959969</v>
+        <v>0.01461662079599629</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1003344230123835</v>
+        <v>0.1003344441797641</v>
       </c>
     </row>
     <row r="8">
@@ -810,13 +810,13 @@
         <v>79.901</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2154550947662716</v>
+        <v>0.2154550947662717</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2077190396678339</v>
+        <v>0.2077190396678332</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06637430047709171</v>
+        <v>0.06637427209568753</v>
       </c>
       <c r="E8" t="n">
         <v>0.1547619047619048</v>
@@ -825,13 +825,13 @@
         <v>0.1666666666666667</v>
       </c>
       <c r="G8" t="n">
-        <v>0.04878842809960496</v>
+        <v>0.04878842809960501</v>
       </c>
       <c r="H8" t="n">
-        <v>0.04105237300116724</v>
+        <v>0.04105237300116657</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1002923661895749</v>
+        <v>0.1002923945709791</v>
       </c>
     </row>
     <row r="9">
@@ -842,10 +842,10 @@
         <v>0.2204628077419719</v>
       </c>
       <c r="C9" t="n">
-        <v>0.2127406016533091</v>
+        <v>0.2127406016533084</v>
       </c>
       <c r="D9" t="n">
-        <v>0.06900445757919055</v>
+        <v>0.06900442849587358</v>
       </c>
       <c r="E9" t="n">
         <v>0.1785714285714286</v>
@@ -857,10 +857,10 @@
         <v>0.02998661726578139</v>
       </c>
       <c r="H9" t="n">
-        <v>0.02226441117711864</v>
+        <v>0.02226441117711797</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1214717328969999</v>
+        <v>0.1214717619803169</v>
       </c>
     </row>
     <row r="10">
@@ -871,10 +871,10 @@
         <v>0.2240393025701286</v>
       </c>
       <c r="C10" t="n">
-        <v>0.2163293575646535</v>
+        <v>0.2163293575646528</v>
       </c>
       <c r="D10" t="n">
-        <v>0.07091121036863203</v>
+        <v>0.0709111807863759</v>
       </c>
       <c r="E10" t="n">
         <v>0.2023809523809524</v>
@@ -886,10 +886,10 @@
         <v>0.009753588284414333</v>
       </c>
       <c r="H10" t="n">
-        <v>0.002043643278939272</v>
+        <v>0.002043643278938551</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1433745039170822</v>
+        <v>0.1433745334993384</v>
       </c>
     </row>
     <row r="11">
@@ -900,10 +900,10 @@
         <v>0.2273461350712963</v>
       </c>
       <c r="C11" t="n">
-        <v>0.2196492423151352</v>
+        <v>0.2196492423151344</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0726951443102684</v>
+        <v>0.07269511426853444</v>
       </c>
       <c r="E11" t="n">
         <v>0.2261904761904762</v>
@@ -912,13 +912,13 @@
         <v>0.2380952380952381</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01074910302394178</v>
+        <v>0.01074910302394183</v>
       </c>
       <c r="H11" t="n">
-        <v>0.01844599578010286</v>
+        <v>0.01844599578010364</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1654000937849697</v>
+        <v>0.1654001238267037</v>
       </c>
     </row>
     <row r="12">
@@ -929,10 +929,10 @@
         <v>0.2366677541784064</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2290162461357511</v>
+        <v>0.2290162461357502</v>
       </c>
       <c r="D12" t="n">
-        <v>0.07783196029649676</v>
+        <v>0.0778319289696798</v>
       </c>
       <c r="E12" t="n">
         <v>0.25</v>
@@ -944,10 +944,10 @@
         <v>0.02523700772635551</v>
       </c>
       <c r="H12" t="n">
-        <v>0.03288851576901086</v>
+        <v>0.03288851576901169</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1840728016082652</v>
+        <v>0.1840728329350821</v>
       </c>
     </row>
     <row r="13">
@@ -958,10 +958,10 @@
         <v>0.2382543055524297</v>
       </c>
       <c r="C13" t="n">
-        <v>0.2306117501956816</v>
+        <v>0.2306117501956809</v>
       </c>
       <c r="D13" t="n">
-        <v>0.07872211340494638</v>
+        <v>0.07872208186097428</v>
       </c>
       <c r="E13" t="n">
         <v>0.2738095238095238</v>
@@ -973,10 +973,10 @@
         <v>0.04745998016185599</v>
       </c>
       <c r="H13" t="n">
-        <v>0.05510253551860411</v>
+        <v>0.05510253551860483</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2069921723093393</v>
+        <v>0.2069922038533114</v>
       </c>
     </row>
     <row r="14">
@@ -987,10 +987,10 @@
         <v>0.2474260685184582</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2398420010791221</v>
+        <v>0.2398420010791213</v>
       </c>
       <c r="D14" t="n">
-        <v>0.08395822882500469</v>
+        <v>0.08395819603521537</v>
       </c>
       <c r="E14" t="n">
         <v>0.2976190476190476</v>
@@ -1002,10 +1002,10 @@
         <v>0.06209774100535131</v>
       </c>
       <c r="H14" t="n">
-        <v>0.06968180844468741</v>
+        <v>0.06968180844468819</v>
       </c>
       <c r="I14" t="n">
-        <v>0.2255655806988048</v>
+        <v>0.2255656134885942</v>
       </c>
     </row>
     <row r="15">
@@ -1016,10 +1016,10 @@
         <v>0.2474865569492724</v>
       </c>
       <c r="C15" t="n">
-        <v>0.2399029125565237</v>
+        <v>0.2399029125565229</v>
       </c>
       <c r="D15" t="n">
-        <v>0.08399327111468681</v>
+        <v>0.08399323831673712</v>
       </c>
       <c r="E15" t="n">
         <v>0.3214285714285715</v>
@@ -1031,10 +1031,10 @@
         <v>0.08584677638406091</v>
       </c>
       <c r="H15" t="n">
-        <v>0.09343042077680963</v>
+        <v>0.09343042077681046</v>
       </c>
       <c r="I15" t="n">
-        <v>0.2493400622186465</v>
+        <v>0.2493400950165962</v>
       </c>
     </row>
     <row r="16">
@@ -1045,10 +1045,10 @@
         <v>0.2917017270447764</v>
       </c>
       <c r="C16" t="n">
-        <v>0.284545658503076</v>
+        <v>0.2845456585030751</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1113835069161228</v>
+        <v>0.1113834683785784</v>
       </c>
       <c r="E16" t="n">
         <v>0.3452380952380952</v>
@@ -1057,13 +1057,13 @@
         <v>0.3571428571428572</v>
       </c>
       <c r="G16" t="n">
-        <v>0.06544113009808072</v>
+        <v>0.06544113009808078</v>
       </c>
       <c r="H16" t="n">
-        <v>0.07259719863978115</v>
+        <v>0.07259719863978203</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2457593502267344</v>
+        <v>0.2457593887642787</v>
       </c>
     </row>
     <row r="17">
@@ -1074,10 +1074,10 @@
         <v>0.2947225247212408</v>
       </c>
       <c r="C17" t="n">
-        <v>0.2876035609587587</v>
+        <v>0.2876035609587578</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1133835257558638</v>
+        <v>0.1133834868444351</v>
       </c>
       <c r="E17" t="n">
         <v>0.3690476190476191</v>
@@ -1089,10 +1089,10 @@
         <v>0.0862298562311401</v>
       </c>
       <c r="H17" t="n">
-        <v>0.09334881999362221</v>
+        <v>0.0933488199936231</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2675688551965171</v>
+        <v>0.2675688941079458</v>
       </c>
     </row>
     <row r="18">
@@ -1100,13 +1100,13 @@
         <v>87.889</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2963388703683681</v>
+        <v>0.296338870368368</v>
       </c>
       <c r="C18" t="n">
-        <v>0.289240138066074</v>
+        <v>0.2892401380660732</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1144604052288724</v>
+        <v>0.1144603661184411</v>
       </c>
       <c r="E18" t="n">
         <v>0.3928571428571428</v>
@@ -1118,10 +1118,10 @@
         <v>0.1084230343935367</v>
       </c>
       <c r="H18" t="n">
-        <v>0.1155217666958308</v>
+        <v>0.1155217666958316</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2903014995330324</v>
+        <v>0.2903015386434636</v>
       </c>
     </row>
     <row r="19">
@@ -1132,10 +1132,10 @@
         <v>0.358722276913348</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3525824291552077</v>
+        <v>0.3525824291552067</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1595804568207833</v>
+        <v>0.1595804106531374</v>
       </c>
       <c r="E19" t="n">
         <v>0.4166666666666667</v>
@@ -1147,10 +1147,10 @@
         <v>0.06984915165808053</v>
       </c>
       <c r="H19" t="n">
-        <v>0.07598899941622089</v>
+        <v>0.07598899941622189</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2689909717506452</v>
+        <v>0.2689910179182911</v>
       </c>
     </row>
     <row r="20">
@@ -1161,10 +1161,10 @@
         <v>0.4189460720623802</v>
       </c>
       <c r="C20" t="n">
-        <v>0.4139921948836415</v>
+        <v>0.4139921948836405</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2096390331449878</v>
+        <v>0.2096389815118543</v>
       </c>
       <c r="E20" t="n">
         <v>0.4404761904761905</v>
@@ -1176,10 +1176,10 @@
         <v>0.03343488031857217</v>
       </c>
       <c r="H20" t="n">
-        <v>0.03838875749731091</v>
+        <v>0.03838875749731191</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2427419192359646</v>
+        <v>0.2427419708690981</v>
       </c>
     </row>
     <row r="21">
@@ -1190,10 +1190,10 @@
         <v>0.4289134727232018</v>
       </c>
       <c r="C21" t="n">
-        <v>0.4241743987264993</v>
+        <v>0.4241743987264983</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2185323097904424</v>
+        <v>0.2185322573982177</v>
       </c>
       <c r="E21" t="n">
         <v>0.4642857142857143</v>
@@ -1205,10 +1205,10 @@
         <v>0.04727700346727431</v>
       </c>
       <c r="H21" t="n">
-        <v>0.05201607746397685</v>
+        <v>0.05201607746397785</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2576581664000338</v>
+        <v>0.2576582187922585</v>
       </c>
     </row>
     <row r="22">
@@ -1219,10 +1219,10 @@
         <v>0.4738477342539273</v>
       </c>
       <c r="C22" t="n">
-        <v>0.4701257915513752</v>
+        <v>0.4701257915513742</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2607463726838885</v>
+        <v>0.2607463174306888</v>
       </c>
       <c r="E22" t="n">
         <v>0.4880952380952381</v>
@@ -1234,10 +1234,10 @@
         <v>0.02615226574607271</v>
       </c>
       <c r="H22" t="n">
-        <v>0.02987420844862476</v>
+        <v>0.02987420844862576</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2392536273161115</v>
+        <v>0.2392536825693112</v>
       </c>
     </row>
     <row r="23">
@@ -1248,10 +1248,10 @@
         <v>0.5321357890372287</v>
       </c>
       <c r="C23" t="n">
-        <v>0.5298154590707826</v>
+        <v>0.5298154590707814</v>
       </c>
       <c r="D23" t="n">
-        <v>0.3206266148195194</v>
+        <v>0.3206265573264406</v>
       </c>
       <c r="E23" t="n">
         <v>0.5119047619047619</v>
@@ -1263,10 +1263,10 @@
         <v>0.008326265227704854</v>
       </c>
       <c r="H23" t="n">
-        <v>0.00600593526125881</v>
+        <v>0.006005935261257589</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2031829089900044</v>
+        <v>0.2031829664830833</v>
       </c>
     </row>
     <row r="24">
@@ -1277,10 +1277,10 @@
         <v>0.5761424783854154</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5749070489036998</v>
+        <v>0.5749070489036989</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3696127641008278</v>
+        <v>0.3696127061080796</v>
       </c>
       <c r="E24" t="n">
         <v>0.5357142857142857</v>
@@ -1292,10 +1292,10 @@
         <v>0.02852343076636776</v>
       </c>
       <c r="H24" t="n">
-        <v>0.02728800128465214</v>
+        <v>0.02728800128465125</v>
       </c>
       <c r="I24" t="n">
-        <v>0.1780062835182198</v>
+        <v>0.1780063415109681</v>
       </c>
     </row>
     <row r="25">
@@ -1306,10 +1306,10 @@
         <v>0.5988018038945421</v>
       </c>
       <c r="C25" t="n">
-        <v>0.5981239651740817</v>
+        <v>0.5981239651740808</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3960879015570422</v>
+        <v>0.3960878437299419</v>
       </c>
       <c r="E25" t="n">
         <v>0.5595238095238095</v>
@@ -1321,10 +1321,10 @@
         <v>0.02737323246597068</v>
       </c>
       <c r="H25" t="n">
-        <v>0.02669539374551033</v>
+        <v>0.02669539374550944</v>
       </c>
       <c r="I25" t="n">
-        <v>0.1753406698715292</v>
+        <v>0.1753407276986295</v>
       </c>
     </row>
     <row r="26">
@@ -1332,13 +1332,13 @@
         <v>119.692</v>
       </c>
       <c r="B26" t="n">
-        <v>0.6118046401611391</v>
+        <v>0.6118046401611392</v>
       </c>
       <c r="C26" t="n">
-        <v>0.6114444222451174</v>
+        <v>0.6114444222451164</v>
       </c>
       <c r="D26" t="n">
-        <v>0.4116615538701797</v>
+        <v>0.4116614962721065</v>
       </c>
       <c r="E26" t="n">
         <v>0.5833333333333334</v>
@@ -1347,13 +1347,13 @@
         <v>0.5952380952380952</v>
       </c>
       <c r="G26" t="n">
-        <v>0.01656654492304388</v>
+        <v>0.01656654492304399</v>
       </c>
       <c r="H26" t="n">
-        <v>0.01620632700702218</v>
+        <v>0.01620632700702118</v>
       </c>
       <c r="I26" t="n">
-        <v>0.1835765413679155</v>
+        <v>0.1835765989659888</v>
       </c>
     </row>
     <row r="27">
@@ -1364,10 +1364,10 @@
         <v>0.616345309525232</v>
       </c>
       <c r="C27" t="n">
-        <v>0.6160954206262322</v>
+        <v>0.6160954206262312</v>
       </c>
       <c r="D27" t="n">
-        <v>0.4171651699873602</v>
+        <v>0.4171651124926196</v>
       </c>
       <c r="E27" t="n">
         <v>0.6071428571428571</v>
@@ -1379,10 +1379,10 @@
         <v>0.002702309522387036</v>
       </c>
       <c r="H27" t="n">
-        <v>0.002952198421386831</v>
+        <v>0.002952198421387831</v>
       </c>
       <c r="I27" t="n">
-        <v>0.2018824490602589</v>
+        <v>0.2018825065549995</v>
       </c>
     </row>
     <row r="28">
@@ -1393,10 +1393,10 @@
         <v>0.6205574342744622</v>
       </c>
       <c r="C28" t="n">
-        <v>0.6204095732058192</v>
+        <v>0.6204095732058181</v>
       </c>
       <c r="D28" t="n">
-        <v>0.4223006743546385</v>
+        <v>0.4223006169666457</v>
       </c>
       <c r="E28" t="n">
         <v>0.6309523809523809</v>
@@ -1408,10 +1408,10 @@
         <v>0.02229970858268071</v>
       </c>
       <c r="H28" t="n">
-        <v>0.02244756965132366</v>
+        <v>0.02244756965132477</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2205564685025044</v>
+        <v>0.2205565258904972</v>
       </c>
     </row>
     <row r="29">
@@ -1419,13 +1419,13 @@
         <v>120.866</v>
       </c>
       <c r="B29" t="n">
-        <v>0.6216847826992838</v>
+        <v>0.621684782699284</v>
       </c>
       <c r="C29" t="n">
-        <v>0.6215641732421128</v>
+        <v>0.621564173242112</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4236800700694461</v>
+        <v>0.4236800127118082</v>
       </c>
       <c r="E29" t="n">
         <v>0.6547619047619048</v>
@@ -1434,13 +1434,13 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="G29" t="n">
-        <v>0.04498188396738279</v>
+        <v>0.04498188396738267</v>
       </c>
       <c r="H29" t="n">
-        <v>0.04510249342455386</v>
+        <v>0.04510249342455463</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2429865965972205</v>
+        <v>0.2429866539548585</v>
       </c>
     </row>
     <row r="30">
@@ -1451,10 +1451,10 @@
         <v>0.6331177416530361</v>
       </c>
       <c r="C30" t="n">
-        <v>0.6332720344205158</v>
+        <v>0.6332720344205147</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4377860971171033</v>
+        <v>0.4377860401101186</v>
       </c>
       <c r="E30" t="n">
         <v>0.6785714285714286</v>
@@ -1466,10 +1466,10 @@
         <v>0.05735844882315433</v>
       </c>
       <c r="H30" t="n">
-        <v>0.05720415605567464</v>
+        <v>0.05720415605567575</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2526900933590872</v>
+        <v>0.2526901503660718</v>
       </c>
     </row>
     <row r="31">
@@ -1480,10 +1480,10 @@
         <v>0.6624454044936983</v>
       </c>
       <c r="C31" t="n">
-        <v>0.663289521042139</v>
+        <v>0.663289521042138</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4749398147344222</v>
+        <v>0.4749397589881968</v>
       </c>
       <c r="E31" t="n">
         <v>0.7023809523809523</v>
@@ -1495,10 +1495,10 @@
         <v>0.05184030979201604</v>
       </c>
       <c r="H31" t="n">
-        <v>0.05099619324357529</v>
+        <v>0.05099619324357629</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2393458995512921</v>
+        <v>0.2393459552975175</v>
       </c>
     </row>
     <row r="32">
@@ -1509,10 +1509,10 @@
         <v>0.6785462256846684</v>
       </c>
       <c r="C32" t="n">
-        <v>0.6797569374910258</v>
+        <v>0.6797569374910249</v>
       </c>
       <c r="D32" t="n">
-        <v>0.495926501942637</v>
+        <v>0.4959264471135255</v>
       </c>
       <c r="E32" t="n">
         <v>0.7261904761904762</v>
@@ -1524,10 +1524,10 @@
         <v>0.05954901241056976</v>
       </c>
       <c r="H32" t="n">
-        <v>0.0583383006042123</v>
+        <v>0.05833830060421319</v>
       </c>
       <c r="I32" t="n">
-        <v>0.2421687361526011</v>
+        <v>0.2421687909817127</v>
       </c>
     </row>
     <row r="33">
@@ -1538,10 +1538,10 @@
         <v>0.6888916987738397</v>
       </c>
       <c r="C33" t="n">
-        <v>0.6903323680001329</v>
+        <v>0.690332368000132</v>
       </c>
       <c r="D33" t="n">
-        <v>0.5096304962457631</v>
+        <v>0.5096304420914597</v>
       </c>
       <c r="E33" t="n">
         <v>0.75</v>
@@ -1553,10 +1553,10 @@
         <v>0.07301306313092215</v>
       </c>
       <c r="H33" t="n">
-        <v>0.07157239390462899</v>
+        <v>0.07157239390462988</v>
       </c>
       <c r="I33" t="n">
-        <v>0.2522742656589988</v>
+        <v>0.2522743198133022</v>
       </c>
     </row>
     <row r="34">
@@ -1567,10 +1567,10 @@
         <v>0.6988391408882454</v>
       </c>
       <c r="C34" t="n">
-        <v>0.70049624332451</v>
+        <v>0.7004962433245092</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5229682951123188</v>
+        <v>0.5229682416705951</v>
       </c>
       <c r="E34" t="n">
         <v>0.7738095238095238</v>
@@ -1582,10 +1582,10 @@
         <v>0.08687514482604031</v>
       </c>
       <c r="H34" t="n">
-        <v>0.08521804238977571</v>
+        <v>0.08521804238977648</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2627459906019669</v>
+        <v>0.2627460440436906</v>
       </c>
     </row>
     <row r="35">
@@ -1596,10 +1596,10 @@
         <v>0.7067520182487361</v>
       </c>
       <c r="C35" t="n">
-        <v>0.708577699139011</v>
+        <v>0.70857769913901</v>
       </c>
       <c r="D35" t="n">
-        <v>0.5336905080675181</v>
+        <v>0.5336904552375852</v>
       </c>
       <c r="E35" t="n">
         <v>0.7976190476190477</v>
@@ -1611,10 +1611,10 @@
         <v>0.1027717912750734</v>
       </c>
       <c r="H35" t="n">
-        <v>0.1009461103847985</v>
+        <v>0.1009461103847995</v>
       </c>
       <c r="I35" t="n">
-        <v>0.2758333014562915</v>
+        <v>0.2758333542862244</v>
       </c>
     </row>
     <row r="36">
@@ -1625,10 +1625,10 @@
         <v>0.7877546663520549</v>
       </c>
       <c r="C36" t="n">
-        <v>0.7910579671496827</v>
+        <v>0.791057967149682</v>
       </c>
       <c r="D36" t="n">
-        <v>0.6491224510566556</v>
+        <v>0.6491224068367332</v>
       </c>
       <c r="E36" t="n">
         <v>0.8214285714285714</v>
@@ -1640,10 +1640,10 @@
         <v>0.04557866698127844</v>
       </c>
       <c r="H36" t="n">
-        <v>0.04227536618365069</v>
+        <v>0.04227536618365135</v>
       </c>
       <c r="I36" t="n">
-        <v>0.1842108822766778</v>
+        <v>0.1842109264966002</v>
       </c>
     </row>
     <row r="37">
@@ -1654,10 +1654,10 @@
         <v>0.8659708447322163</v>
       </c>
       <c r="C37" t="n">
-        <v>0.8700062222782761</v>
+        <v>0.8700062222782756</v>
       </c>
       <c r="D37" t="n">
-        <v>0.770249849312685</v>
+        <v>0.7702498176161161</v>
       </c>
       <c r="E37" t="n">
         <v>0.8452380952380952</v>
@@ -1669,10 +1669,10 @@
         <v>0.00882798758935921</v>
       </c>
       <c r="H37" t="n">
-        <v>0.01286336513541897</v>
+        <v>0.01286336513541853</v>
       </c>
       <c r="I37" t="n">
-        <v>0.08689300783017206</v>
+        <v>0.08689303952674099</v>
       </c>
     </row>
     <row r="38">
@@ -1683,10 +1683,10 @@
         <v>0.8901830651801689</v>
       </c>
       <c r="C38" t="n">
-        <v>0.8942157470270049</v>
+        <v>0.8942157470270045</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8096576330506836</v>
+        <v>0.8096576061010571</v>
       </c>
       <c r="E38" t="n">
         <v>0.8690476190476191</v>
@@ -1698,10 +1698,10 @@
         <v>0.009230684227787944</v>
       </c>
       <c r="H38" t="n">
-        <v>0.01326336607462397</v>
+        <v>0.01326336607462353</v>
       </c>
       <c r="I38" t="n">
-        <v>0.07129474790169732</v>
+        <v>0.07129477485132385</v>
       </c>
     </row>
     <row r="39">
@@ -1712,10 +1712,10 @@
         <v>0.913458139722889</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9173353034810199</v>
+        <v>0.9173353034810195</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8484021126087865</v>
+        <v>0.8484020906211744</v>
       </c>
       <c r="E39" t="n">
         <v>0.8928571428571429</v>
@@ -1727,10 +1727,10 @@
         <v>0.008696234960984262</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01257339871911511</v>
+        <v>0.01257339871911478</v>
       </c>
       <c r="I39" t="n">
-        <v>0.05635979215311826</v>
+        <v>0.05635981414073032</v>
       </c>
     </row>
     <row r="40">
@@ -1741,10 +1741,10 @@
         <v>0.9247625945204265</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9284958333822537</v>
+        <v>0.9284958333822534</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8675299391413916</v>
+        <v>0.8675299197071487</v>
       </c>
       <c r="E40" t="n">
         <v>0.9166666666666666</v>
@@ -1756,10 +1756,10 @@
         <v>0.003808834051002075</v>
       </c>
       <c r="H40" t="n">
-        <v>7.559518917488184e-05</v>
+        <v>7.559518917521491e-05</v>
       </c>
       <c r="I40" t="n">
-        <v>0.06104148943003695</v>
+        <v>0.06104150886427995</v>
       </c>
     </row>
     <row r="41">
@@ -1770,10 +1770,10 @@
         <v>0.9714602391574156</v>
       </c>
       <c r="C41" t="n">
-        <v>0.9738532505794389</v>
+        <v>0.9738532505794388</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9488088073313276</v>
+        <v>0.9488087994715971</v>
       </c>
       <c r="E41" t="n">
         <v>0.9404761904761905</v>
@@ -1785,10 +1785,10 @@
         <v>0.01907928677646331</v>
       </c>
       <c r="H41" t="n">
-        <v>0.02147229819848662</v>
+        <v>0.02147229819848651</v>
       </c>
       <c r="I41" t="n">
-        <v>0.003572145049624775</v>
+        <v>0.003572152909355197</v>
       </c>
     </row>
     <row r="42">
@@ -1799,10 +1799,10 @@
         <v>0.9805243881396879</v>
       </c>
       <c r="C42" t="n">
-        <v>0.9824242202613794</v>
+        <v>0.9824242202613793</v>
       </c>
       <c r="D42" t="n">
-        <v>0.9650394847599911</v>
+        <v>0.9650394793462128</v>
       </c>
       <c r="E42" t="n">
         <v>0.9642857142857143</v>
@@ -1814,10 +1814,10 @@
         <v>0.004333911949211733</v>
       </c>
       <c r="H42" t="n">
-        <v>0.006233744070903269</v>
+        <v>0.006233744070903158</v>
       </c>
       <c r="I42" t="n">
-        <v>0.01115099143048504</v>
+        <v>0.01115099684426335</v>
       </c>
     </row>
     <row r="43">
@@ -1831,7 +1831,7 @@
         <v>0.9863681276060511</v>
       </c>
       <c r="D43" t="n">
-        <v>0.972652530959374</v>
+        <v>0.9726525267077475</v>
       </c>
       <c r="E43" t="n">
         <v>0.9880952380952381</v>
@@ -1846,7 +1846,7 @@
         <v>0.01363187239394892</v>
       </c>
       <c r="I43" t="n">
-        <v>0.02734746904062602</v>
+        <v>0.02734747329225251</v>
       </c>
     </row>
   </sheetData>
@@ -1911,7 +1911,7 @@
         <v>0.008647973303246981</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002250629251403668</v>
+        <v>0.002250627665240272</v>
       </c>
       <c r="E2" t="n">
         <v>0.01063829787234043</v>
@@ -1931,7 +1931,7 @@
         <v>0.05882555545401921</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01620181912852355</v>
+        <v>0.01620181140707962</v>
       </c>
       <c r="E3" t="n">
         <v>0.03191489361702127</v>
@@ -1951,7 +1951,7 @@
         <v>0.1341138410239009</v>
       </c>
       <c r="D4" t="n">
-        <v>0.04430757627959986</v>
+        <v>0.04430756031642659</v>
       </c>
       <c r="E4" t="n">
         <v>0.05319148936170213</v>
@@ -1971,7 +1971,7 @@
         <v>0.142733292181175</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0480306685174364</v>
+        <v>0.0480306516608922</v>
       </c>
       <c r="E5" t="n">
         <v>0.07446808510638298</v>
@@ -1991,7 +1991,7 @@
         <v>0.1520522487048782</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05216881296865133</v>
+        <v>0.05216879515822161</v>
       </c>
       <c r="E6" t="n">
         <v>0.09574468085106383</v>
@@ -2011,7 +2011,7 @@
         <v>0.1546523522260774</v>
       </c>
       <c r="D7" t="n">
-        <v>0.05334423456747039</v>
+        <v>0.05334421649315065</v>
       </c>
       <c r="E7" t="n">
         <v>0.1170212765957447</v>
@@ -2031,7 +2031,7 @@
         <v>0.2019315193222429</v>
       </c>
       <c r="D8" t="n">
-        <v>0.07628552214743629</v>
+        <v>0.07628549945463689</v>
       </c>
       <c r="E8" t="n">
         <v>0.1382978723404255</v>
@@ -2051,7 +2051,7 @@
         <v>0.2066460014159929</v>
       </c>
       <c r="D9" t="n">
-        <v>0.07873490195711833</v>
+        <v>0.07873487882334494</v>
       </c>
       <c r="E9" t="n">
         <v>0.1595744680851064</v>
@@ -2071,7 +2071,7 @@
         <v>0.210014502505086</v>
       </c>
       <c r="D10" t="n">
-        <v>0.08050285629959085</v>
+        <v>0.08050283285301391</v>
       </c>
       <c r="E10" t="n">
         <v>0.1808510638297872</v>
@@ -2091,7 +2091,7 @@
         <v>0.2131300951398636</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08215132139636608</v>
+        <v>0.08215129766217272</v>
       </c>
       <c r="E11" t="n">
         <v>0.2021276595744681</v>
@@ -2111,7 +2111,7 @@
         <v>0.2219182424646712</v>
       </c>
       <c r="D12" t="n">
-        <v>0.08686969612340947</v>
+        <v>0.08686967158685824</v>
       </c>
       <c r="E12" t="n">
         <v>0.2234042553191489</v>
@@ -2131,7 +2131,7 @@
         <v>0.2234148307080164</v>
       </c>
       <c r="D13" t="n">
-        <v>0.08768329734648726</v>
+        <v>0.08768327267462431</v>
       </c>
       <c r="E13" t="n">
         <v>0.2446808510638298</v>
@@ -2151,7 +2151,7 @@
         <v>0.2320713514120815</v>
       </c>
       <c r="D14" t="n">
-        <v>0.09244682132472171</v>
+        <v>0.09244679587788401</v>
       </c>
       <c r="E14" t="n">
         <v>0.2659574468085106</v>
@@ -2165,13 +2165,13 @@
         <v>83.13500000000001</v>
       </c>
       <c r="B15" t="n">
-        <v>0.2607824823460791</v>
+        <v>0.2607824823460792</v>
       </c>
       <c r="C15" t="n">
         <v>0.232128469330987</v>
       </c>
       <c r="D15" t="n">
-        <v>0.09247857786826504</v>
+        <v>0.09247855241635777</v>
       </c>
       <c r="E15" t="n">
         <v>0.2872340425531915</v>
@@ -2191,7 +2191,7 @@
         <v>0.273980040406938</v>
       </c>
       <c r="D16" t="n">
-        <v>0.116894286702627</v>
+        <v>0.116894257697054</v>
       </c>
       <c r="E16" t="n">
         <v>0.3085106382978723</v>
@@ -2211,7 +2211,7 @@
         <v>0.2768468781645126</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1186506473039972</v>
+        <v>0.1186506180671637</v>
       </c>
       <c r="E17" t="n">
         <v>0.3297872340425532</v>
@@ -2231,7 +2231,7 @@
         <v>0.2783812510755337</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1195951011991904</v>
+        <v>0.1195950718392458</v>
       </c>
       <c r="E18" t="n">
         <v>0.351063829787234</v>
@@ -2248,10 +2248,10 @@
         <v>0.3478922977144504</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3235742483507528</v>
+        <v>0.3235742483507529</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1488002803577517</v>
+        <v>0.148800247586484</v>
       </c>
       <c r="E19" t="n">
         <v>0.3723404255319149</v>
@@ -2271,7 +2271,7 @@
         <v>0.3378262024089898</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1585695801424694</v>
+        <v>0.1585695463852686</v>
       </c>
       <c r="E20" t="n">
         <v>0.3936170212765958</v>
@@ -2291,7 +2291,7 @@
         <v>0.3956598256175535</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2009994500814186</v>
+        <v>0.2009994128008815</v>
       </c>
       <c r="E21" t="n">
         <v>0.4148936170212766</v>
@@ -2311,7 +2311,7 @@
         <v>0.4041267711187648</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2075906597592331</v>
+        <v>0.2075906220304927</v>
       </c>
       <c r="E22" t="n">
         <v>0.4361702127659575</v>
@@ -2331,7 +2331,7 @@
         <v>0.4052771216093275</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2084937220810601</v>
+        <v>0.2084936842928131</v>
       </c>
       <c r="E23" t="n">
         <v>0.4574468085106383</v>
@@ -2351,7 +2351,7 @@
         <v>0.4251460282350601</v>
       </c>
       <c r="D24" t="n">
-        <v>0.2243781817854163</v>
+        <v>0.2243781430226966</v>
       </c>
       <c r="E24" t="n">
         <v>0.4787234042553192</v>
@@ -2371,7 +2371,7 @@
         <v>0.4488041729174384</v>
       </c>
       <c r="D25" t="n">
-        <v>0.2440049527907195</v>
+        <v>0.2440049130026789</v>
       </c>
       <c r="E25" t="n">
         <v>0.5</v>
@@ -2391,7 +2391,7 @@
         <v>0.5057134557002478</v>
       </c>
       <c r="D26" t="n">
-        <v>0.2944593107119439</v>
+        <v>0.2944592690945303</v>
       </c>
       <c r="E26" t="n">
         <v>0.5212765957446809</v>
@@ -2411,7 +2411,7 @@
         <v>0.5490463147091303</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3360436877158089</v>
+        <v>0.3360436453527507</v>
       </c>
       <c r="E27" t="n">
         <v>0.5425531914893617</v>
@@ -2431,7 +2431,7 @@
         <v>0.5714930010300717</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3586987757928882</v>
+        <v>0.3586987332791397</v>
       </c>
       <c r="E28" t="n">
         <v>0.5638297872340425</v>
@@ -2451,7 +2451,7 @@
         <v>0.5844175829457535</v>
       </c>
       <c r="D29" t="n">
-        <v>0.372097060982836</v>
+        <v>0.3720970184585175</v>
       </c>
       <c r="E29" t="n">
         <v>0.5851063829787234</v>
@@ -2471,7 +2471,7 @@
         <v>0.5889386867937221</v>
       </c>
       <c r="D30" t="n">
-        <v>0.3768457383615593</v>
+        <v>0.3768456958469866</v>
       </c>
       <c r="E30" t="n">
         <v>0.6063829787234043</v>
@@ -2491,7 +2491,7 @@
         <v>0.5931363181348163</v>
       </c>
       <c r="D31" t="n">
-        <v>0.3812835925995336</v>
+        <v>0.3812835501003237</v>
       </c>
       <c r="E31" t="n">
         <v>0.6276595744680851</v>
@@ -2511,7 +2511,7 @@
         <v>0.5942603893901224</v>
       </c>
       <c r="D32" t="n">
-        <v>0.3824767384380667</v>
+        <v>0.3824766959440085</v>
       </c>
       <c r="E32" t="n">
         <v>0.648936170212766</v>
@@ -2531,7 +2531,7 @@
         <v>0.6056746767228171</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3947066989319746</v>
+        <v>0.3947066565152969</v>
       </c>
       <c r="E33" t="n">
         <v>0.6702127659574468</v>
@@ -2548,10 +2548,10 @@
         <v>0.633494986614397</v>
       </c>
       <c r="C34" t="n">
-        <v>0.6350802116839612</v>
+        <v>0.6350802116839613</v>
       </c>
       <c r="D34" t="n">
-        <v>0.4271878229029907</v>
+        <v>0.4271877809010318</v>
       </c>
       <c r="E34" t="n">
         <v>0.6914893617021277</v>
@@ -2571,7 +2571,7 @@
         <v>0.6513048276183671</v>
       </c>
       <c r="D35" t="n">
-        <v>0.4457247120557</v>
+        <v>0.4457246704198679</v>
       </c>
       <c r="E35" t="n">
         <v>0.7127659574468085</v>
@@ -2588,10 +2588,10 @@
         <v>0.6578888628940529</v>
       </c>
       <c r="C36" t="n">
-        <v>0.661761815202753</v>
+        <v>0.6617618152027531</v>
       </c>
       <c r="D36" t="n">
-        <v>0.457909723023923</v>
+        <v>0.457909681677546</v>
       </c>
       <c r="E36" t="n">
         <v>0.7340425531914894</v>
@@ -2611,7 +2611,7 @@
         <v>0.6718409513999472</v>
       </c>
       <c r="D37" t="n">
-        <v>0.4698339152189661</v>
+        <v>0.4698338741921476</v>
       </c>
       <c r="E37" t="n">
         <v>0.7553191489361702</v>
@@ -2628,10 +2628,10 @@
         <v>0.674444341941868</v>
       </c>
       <c r="C38" t="n">
-        <v>0.6798200263440446</v>
+        <v>0.6798200263440445</v>
       </c>
       <c r="D38" t="n">
-        <v>0.4794003394046355</v>
+        <v>0.4794002986595259</v>
       </c>
       <c r="E38" t="n">
         <v>0.776595744680851</v>
@@ -2651,7 +2651,7 @@
         <v>0.6798762327767303</v>
       </c>
       <c r="D39" t="n">
-        <v>0.479468128411829</v>
+        <v>0.4794680876687949</v>
       </c>
       <c r="E39" t="n">
         <v>0.7978723404255319</v>
@@ -2665,13 +2665,13 @@
         <v>145.328</v>
       </c>
       <c r="B40" t="n">
-        <v>0.7515768552681846</v>
+        <v>0.7515768552681845</v>
       </c>
       <c r="C40" t="n">
         <v>0.7631433910939411</v>
       </c>
       <c r="D40" t="n">
-        <v>0.5863925041399223</v>
+        <v>0.586392467957342</v>
       </c>
       <c r="E40" t="n">
         <v>0.8191489361702128</v>
@@ -2691,7 +2691,7 @@
         <v>0.8457813707196551</v>
       </c>
       <c r="D41" t="n">
-        <v>0.7070534642194947</v>
+        <v>0.7070534358858468</v>
       </c>
       <c r="E41" t="n">
         <v>0.8404255319148937</v>
@@ -2711,7 +2711,7 @@
         <v>0.8719818808477633</v>
       </c>
       <c r="D42" t="n">
-        <v>0.7489630714064581</v>
+        <v>0.7489630463789788</v>
       </c>
       <c r="E42" t="n">
         <v>0.8617021276595744</v>
@@ -2731,7 +2731,7 @@
         <v>0.8975448382798568</v>
       </c>
       <c r="D43" t="n">
-        <v>0.7919076824825243</v>
+        <v>0.7919076611241076</v>
       </c>
       <c r="E43" t="n">
         <v>0.8829787234042553</v>
@@ -2751,7 +2751,7 @@
         <v>0.9101224683955472</v>
       </c>
       <c r="D44" t="n">
-        <v>0.8138844757799718</v>
+        <v>0.8138844564042845</v>
       </c>
       <c r="E44" t="n">
         <v>0.9042553191489362</v>
@@ -2771,7 +2771,7 @@
         <v>0.9637582826086037</v>
       </c>
       <c r="D45" t="n">
-        <v>0.9158965491507127</v>
+        <v>0.9158965398491125</v>
       </c>
       <c r="E45" t="n">
         <v>0.925531914893617</v>
@@ -2791,7 +2791,7 @@
         <v>0.9746781025785772</v>
       </c>
       <c r="D46" t="n">
-        <v>0.9390175881448769</v>
+        <v>0.9390175813147288</v>
       </c>
       <c r="E46" t="n">
         <v>0.9468085106382979</v>
@@ -2811,7 +2811,7 @@
         <v>0.9798683770756452</v>
       </c>
       <c r="D47" t="n">
-        <v>0.9504529953029421</v>
+        <v>0.9504529897195735</v>
       </c>
       <c r="E47" t="n">
         <v>0.9680851063829787</v>
@@ -2831,7 +2831,7 @@
         <v>0.9976031575415124</v>
       </c>
       <c r="D48" t="n">
-        <v>0.9932795317173051</v>
+        <v>0.993279530943031</v>
       </c>
       <c r="E48" t="n">
         <v>0.9893617021276596</v>
@@ -2914,10 +2914,10 @@
         <v>0.04532667197068628</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03836409679582967</v>
+        <v>0.0383640967958297</v>
       </c>
       <c r="D2" t="n">
-        <v>0.005149288448955172</v>
+        <v>0.005149284065766067</v>
       </c>
       <c r="E2" t="n">
         <v>0.0119047619047619</v>
@@ -2929,10 +2929,10 @@
         <v>0.02151714816116247</v>
       </c>
       <c r="H2" t="n">
-        <v>0.01455457298630586</v>
+        <v>0.01455457298630589</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01866023536056863</v>
+        <v>0.01866023974375774</v>
       </c>
     </row>
     <row r="3">
@@ -2946,7 +2946,7 @@
         <v>0.05811264135190177</v>
       </c>
       <c r="D3" t="n">
-        <v>0.009450336462307042</v>
+        <v>0.009450329345005384</v>
       </c>
       <c r="E3" t="n">
         <v>0.03571428571428571</v>
@@ -2961,7 +2961,7 @@
         <v>0.01049359373285415</v>
       </c>
       <c r="I3" t="n">
-        <v>0.03816871115674057</v>
+        <v>0.03816871827404223</v>
       </c>
     </row>
     <row r="4">
@@ -2972,10 +2972,10 @@
         <v>0.1170442383146548</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1060379755131709</v>
+        <v>0.106037975513171</v>
       </c>
       <c r="D4" t="n">
-        <v>0.02352257270241736</v>
+        <v>0.02352255845239084</v>
       </c>
       <c r="E4" t="n">
         <v>0.05952380952380952</v>
@@ -2987,10 +2987,10 @@
         <v>0.0456156668860834</v>
       </c>
       <c r="H4" t="n">
-        <v>0.03460940408459948</v>
+        <v>0.03460940408459953</v>
       </c>
       <c r="I4" t="n">
-        <v>0.04790599872615407</v>
+        <v>0.04790601297618059</v>
       </c>
     </row>
     <row r="5">
@@ -3001,10 +3001,10 @@
         <v>0.1215376824557723</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1103972762585637</v>
+        <v>0.1103972762585638</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02503863733737148</v>
+        <v>0.02503862242156779</v>
       </c>
       <c r="E5" t="n">
         <v>0.08333333333333333</v>
@@ -3016,10 +3016,10 @@
         <v>0.02629958721767706</v>
       </c>
       <c r="H5" t="n">
-        <v>0.01515918102046843</v>
+        <v>0.01515918102046854</v>
       </c>
       <c r="I5" t="n">
-        <v>0.07019945790072375</v>
+        <v>0.07019947281652744</v>
       </c>
     </row>
     <row r="6">
@@ -3030,10 +3030,10 @@
         <v>0.1392886890801395</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1277152932898553</v>
+        <v>0.1277152932898554</v>
       </c>
       <c r="D6" t="n">
-        <v>0.03142979156554484</v>
+        <v>0.03142977399679556</v>
       </c>
       <c r="E6" t="n">
         <v>0.1071428571428571</v>
@@ -3045,10 +3045,10 @@
         <v>0.02024107003252043</v>
       </c>
       <c r="H6" t="n">
-        <v>0.008667674242236273</v>
+        <v>0.008667674242236328</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0876178274820742</v>
+        <v>0.08761784505082348</v>
       </c>
     </row>
     <row r="7">
@@ -3062,7 +3062,7 @@
         <v>0.1302506944650978</v>
       </c>
       <c r="D7" t="n">
-        <v>0.03241413309385233</v>
+        <v>0.03241411513636291</v>
       </c>
       <c r="E7" t="n">
         <v>0.130952380952381</v>
@@ -3074,10 +3074,10 @@
         <v>0.0009819862210175279</v>
       </c>
       <c r="H7" t="n">
-        <v>0.01260644839204506</v>
+        <v>0.012606448392045</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1104430097632905</v>
+        <v>0.1104430277207799</v>
       </c>
     </row>
     <row r="8">
@@ -3091,7 +3091,7 @@
         <v>0.1652977376639957</v>
       </c>
       <c r="D8" t="n">
-        <v>0.04725749262546157</v>
+        <v>0.04725746932314587</v>
       </c>
       <c r="E8" t="n">
         <v>0.1547619047619048</v>
@@ -3106,7 +3106,7 @@
         <v>0.00136892900267091</v>
       </c>
       <c r="I8" t="n">
-        <v>0.1194091740412051</v>
+        <v>0.1194091973435208</v>
       </c>
     </row>
     <row r="9">
@@ -3114,13 +3114,13 @@
         <v>79.901</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1894088382927069</v>
+        <v>0.189408838292707</v>
       </c>
       <c r="C9" t="n">
         <v>0.1773034937306383</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05286074548738718</v>
+        <v>0.05286072037905183</v>
       </c>
       <c r="E9" t="n">
         <v>0.1785714285714286</v>
@@ -3129,13 +3129,13 @@
         <v>0.1904761904761905</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001067352183483528</v>
+        <v>0.001067352183483472</v>
       </c>
       <c r="H9" t="n">
-        <v>0.01317269674555221</v>
+        <v>0.01317269674555216</v>
       </c>
       <c r="I9" t="n">
-        <v>0.1376154449888033</v>
+        <v>0.1376154700971386</v>
       </c>
     </row>
     <row r="10">
@@ -3146,10 +3146,10 @@
         <v>0.1976181584774409</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1855062400867626</v>
+        <v>0.1855062400867627</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05683782106451212</v>
+        <v>0.05683779473321186</v>
       </c>
       <c r="E10" t="n">
         <v>0.2023809523809524</v>
@@ -3161,10 +3161,10 @@
         <v>0.01666755580827337</v>
       </c>
       <c r="H10" t="n">
-        <v>0.02877947419895169</v>
+        <v>0.02877947419895158</v>
       </c>
       <c r="I10" t="n">
-        <v>0.1574478932212021</v>
+        <v>0.1574479195525024</v>
       </c>
     </row>
     <row r="11">
@@ -3178,7 +3178,7 @@
         <v>0.197659134327423</v>
       </c>
       <c r="D11" t="n">
-        <v>0.062949510881328</v>
+        <v>0.06294948275732037</v>
       </c>
       <c r="E11" t="n">
         <v>0.2261904761904762</v>
@@ -3190,10 +3190,10 @@
         <v>0.02834976465640349</v>
       </c>
       <c r="H11" t="n">
-        <v>0.04043610376781509</v>
+        <v>0.04043610376781503</v>
       </c>
       <c r="I11" t="n">
-        <v>0.1751457272139101</v>
+        <v>0.1751457553379177</v>
       </c>
     </row>
     <row r="12">
@@ -3201,13 +3201,13 @@
         <v>83.129</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2201222857493693</v>
+        <v>0.2201222857493692</v>
       </c>
       <c r="C12" t="n">
-        <v>0.2080891577778649</v>
+        <v>0.208089157777865</v>
       </c>
       <c r="D12" t="n">
-        <v>0.06840151846568185</v>
+        <v>0.06840148882376811</v>
       </c>
       <c r="E12" t="n">
         <v>0.25</v>
@@ -3216,13 +3216,13 @@
         <v>0.2619047619047619</v>
       </c>
       <c r="G12" t="n">
-        <v>0.04178247615539266</v>
+        <v>0.04178247615539271</v>
       </c>
       <c r="H12" t="n">
-        <v>0.05381560412689701</v>
+        <v>0.05381560412689695</v>
       </c>
       <c r="I12" t="n">
-        <v>0.1935032434390801</v>
+        <v>0.1935032730809938</v>
       </c>
     </row>
     <row r="13">
@@ -3236,7 +3236,7 @@
         <v>0.2081479938294423</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0684328111716121</v>
+        <v>0.06843278152119431</v>
       </c>
       <c r="E13" t="n">
         <v>0.2738095238095238</v>
@@ -3245,13 +3245,13 @@
         <v>0.2857142857142857</v>
       </c>
       <c r="G13" t="n">
-        <v>0.06553354175863346</v>
+        <v>0.06553354175863352</v>
       </c>
       <c r="H13" t="n">
         <v>0.07756629188484343</v>
       </c>
       <c r="I13" t="n">
-        <v>0.2172814745426736</v>
+        <v>0.2172815041930914</v>
       </c>
     </row>
     <row r="14">
@@ -3265,7 +3265,7 @@
         <v>0.2547055712978784</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0950555053948795</v>
+        <v>0.09505546925581394</v>
       </c>
       <c r="E14" t="n">
         <v>0.2976190476190476</v>
@@ -3277,10 +3277,10 @@
         <v>0.04332581933786928</v>
       </c>
       <c r="H14" t="n">
-        <v>0.05481823822593118</v>
+        <v>0.05481823822593113</v>
       </c>
       <c r="I14" t="n">
-        <v>0.21446830412893</v>
+        <v>0.2144683402679956</v>
       </c>
     </row>
     <row r="15">
@@ -3294,7 +3294,7 @@
         <v>0.2563190198611066</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0960438851607343</v>
+        <v>0.09604384880640364</v>
       </c>
       <c r="E15" t="n">
         <v>0.3214285714285715</v>
@@ -3309,7 +3309,7 @@
         <v>0.0770143134722267</v>
       </c>
       <c r="I15" t="n">
-        <v>0.237289448172599</v>
+        <v>0.2372894845269297</v>
       </c>
     </row>
     <row r="16">
@@ -3323,7 +3323,7 @@
         <v>0.272275423034344</v>
       </c>
       <c r="D16" t="n">
-        <v>0.1060521333858874</v>
+        <v>0.1060520949416104</v>
       </c>
       <c r="E16" t="n">
         <v>0.3452380952380952</v>
@@ -3338,7 +3338,7 @@
         <v>0.08486743410851311</v>
       </c>
       <c r="I16" t="n">
-        <v>0.2510907237569697</v>
+        <v>0.2510907622012467</v>
       </c>
     </row>
     <row r="17">
@@ -3352,7 +3352,7 @@
         <v>0.319488115586023</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1381153188597321</v>
+        <v>0.1381152746866954</v>
       </c>
       <c r="E17" t="n">
         <v>0.3690476190476191</v>
@@ -3367,7 +3367,7 @@
         <v>0.06146426536635791</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2428370620926489</v>
+        <v>0.2428371062656855</v>
       </c>
     </row>
     <row r="18">
@@ -3381,7 +3381,7 @@
         <v>0.3322720718746855</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1474179783484493</v>
+        <v>0.1474179327525842</v>
       </c>
       <c r="E18" t="n">
         <v>0.3928571428571428</v>
@@ -3396,7 +3396,7 @@
         <v>0.07248983288721922</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2573439264134555</v>
+        <v>0.2573439720093205</v>
       </c>
     </row>
     <row r="19">
@@ -3407,10 +3407,10 @@
         <v>0.3901761674654039</v>
       </c>
       <c r="C19" t="n">
-        <v>0.3819107160416727</v>
+        <v>0.3819107160416728</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1860002321232449</v>
+        <v>0.1860001815798042</v>
       </c>
       <c r="E19" t="n">
         <v>0.4166666666666667</v>
@@ -3422,10 +3422,10 @@
         <v>0.03839526110602465</v>
       </c>
       <c r="H19" t="n">
-        <v>0.04666071252975584</v>
+        <v>0.04666071252975579</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2425711964481836</v>
+        <v>0.2425712469916244</v>
       </c>
     </row>
     <row r="20">
@@ -3439,7 +3439,7 @@
         <v>0.3923589851210169</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1946144512638833</v>
+        <v>0.1946143998030467</v>
       </c>
       <c r="E20" t="n">
         <v>0.4404761904761905</v>
@@ -3448,13 +3448,13 @@
         <v>0.4523809523809524</v>
       </c>
       <c r="G20" t="n">
-        <v>0.05209899087866443</v>
+        <v>0.05209899087866438</v>
       </c>
       <c r="H20" t="n">
-        <v>0.06002196725993553</v>
+        <v>0.06002196725993547</v>
       </c>
       <c r="I20" t="n">
-        <v>0.2577665011170691</v>
+        <v>0.2577665525779057</v>
       </c>
     </row>
     <row r="21">
@@ -3468,7 +3468,7 @@
         <v>0.3987914740456758</v>
       </c>
       <c r="D21" t="n">
-        <v>0.2000023177300909</v>
+        <v>0.2000022657269522</v>
       </c>
       <c r="E21" t="n">
         <v>0.4642857142857143</v>
@@ -3483,7 +3483,7 @@
         <v>0.07739900214480039</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2761881584603852</v>
+        <v>0.276188210463524</v>
       </c>
     </row>
     <row r="22">
@@ -3497,7 +3497,7 @@
         <v>0.5021535662662</v>
       </c>
       <c r="D22" t="n">
-        <v>0.2952905999659242</v>
+        <v>0.2952905417743604</v>
       </c>
       <c r="E22" t="n">
         <v>0.4880952380952381</v>
@@ -3512,7 +3512,7 @@
         <v>0.002153566266200002</v>
       </c>
       <c r="I22" t="n">
-        <v>0.2047094000340758</v>
+        <v>0.2047094582256396</v>
       </c>
     </row>
     <row r="23">
@@ -3526,7 +3526,7 @@
         <v>0.5061883472220433</v>
       </c>
       <c r="D23" t="n">
-        <v>0.2993392033372095</v>
+        <v>0.2993391450063462</v>
       </c>
       <c r="E23" t="n">
         <v>0.5119047619047619</v>
@@ -3541,7 +3541,7 @@
         <v>0.01762117658748052</v>
       </c>
       <c r="I23" t="n">
-        <v>0.2244703204723143</v>
+        <v>0.2244703788031776</v>
       </c>
     </row>
     <row r="24">
@@ -3552,10 +3552,10 @@
         <v>0.5517670863942875</v>
       </c>
       <c r="C24" t="n">
-        <v>0.5496795370978785</v>
+        <v>0.5496795370978784</v>
       </c>
       <c r="D24" t="n">
-        <v>0.3445311813821007</v>
+        <v>0.3445311220712378</v>
       </c>
       <c r="E24" t="n">
         <v>0.5357142857142857</v>
@@ -3567,10 +3567,10 @@
         <v>0.004148038775239837</v>
       </c>
       <c r="H24" t="n">
-        <v>0.002060489478830863</v>
+        <v>0.002060489478830752</v>
       </c>
       <c r="I24" t="n">
-        <v>0.203087866236947</v>
+        <v>0.2030879255478099</v>
       </c>
     </row>
     <row r="25">
@@ -3584,7 +3584,7 @@
         <v>0.5742775837190234</v>
       </c>
       <c r="D25" t="n">
-        <v>0.3713444531250806</v>
+        <v>0.3713443936945287</v>
       </c>
       <c r="E25" t="n">
         <v>0.5595238095238095</v>
@@ -3599,7 +3599,7 @@
         <v>0.00284901229045198</v>
       </c>
       <c r="I25" t="n">
-        <v>0.2000841183034908</v>
+        <v>0.2000841777340427</v>
       </c>
     </row>
     <row r="26">
@@ -3610,10 +3610,10 @@
         <v>0.5937591835832153</v>
       </c>
       <c r="C26" t="n">
-        <v>0.5933716865863164</v>
+        <v>0.5933716865863163</v>
       </c>
       <c r="D26" t="n">
-        <v>0.3927808303108698</v>
+        <v>0.3927807710108728</v>
       </c>
       <c r="E26" t="n">
         <v>0.5833333333333334</v>
@@ -3625,10 +3625,10 @@
         <v>0.0014789116548799</v>
       </c>
       <c r="H26" t="n">
-        <v>0.001866408651778784</v>
+        <v>0.001866408651778895</v>
       </c>
       <c r="I26" t="n">
-        <v>0.2024572649272254</v>
+        <v>0.2024573242272224</v>
       </c>
     </row>
     <row r="27">
@@ -3639,10 +3639,10 @@
         <v>0.5981722965883877</v>
       </c>
       <c r="C27" t="n">
-        <v>0.5979618742790413</v>
+        <v>0.5979618742790412</v>
       </c>
       <c r="D27" t="n">
-        <v>0.3980152078384691</v>
+        <v>0.3980151485994688</v>
       </c>
       <c r="E27" t="n">
         <v>0.6071428571428571</v>
@@ -3654,10 +3654,10 @@
         <v>0.0208753224592314</v>
       </c>
       <c r="H27" t="n">
-        <v>0.02108574476857772</v>
+        <v>0.02108574476857783</v>
       </c>
       <c r="I27" t="n">
-        <v>0.22103241120915</v>
+        <v>0.2210324704481503</v>
       </c>
     </row>
     <row r="28">
@@ -3671,7 +3671,7 @@
         <v>0.5991907647586431</v>
       </c>
       <c r="D28" t="n">
-        <v>0.3994218971419746</v>
+        <v>0.3994218379212686</v>
       </c>
       <c r="E28" t="n">
         <v>0.6309523809523809</v>
@@ -3686,7 +3686,7 @@
         <v>0.04366637809849983</v>
       </c>
       <c r="I28" t="n">
-        <v>0.2434352457151683</v>
+        <v>0.2434353049358743</v>
       </c>
     </row>
     <row r="29">
@@ -3700,7 +3700,7 @@
         <v>0.6437100133386293</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4519034554790752</v>
+        <v>0.4519033974899686</v>
       </c>
       <c r="E29" t="n">
         <v>0.6547619047619048</v>
@@ -3715,7 +3715,7 @@
         <v>0.02295665332803731</v>
       </c>
       <c r="I29" t="n">
-        <v>0.2147632111875914</v>
+        <v>0.2147632691766981</v>
       </c>
     </row>
     <row r="30">
@@ -3729,7 +3729,7 @@
         <v>0.6452059137521032</v>
       </c>
       <c r="D30" t="n">
-        <v>0.4537183954027312</v>
+        <v>0.4537183374745307</v>
       </c>
       <c r="E30" t="n">
         <v>0.6785714285714286</v>
@@ -3744,7 +3744,7 @@
         <v>0.04527027672408723</v>
       </c>
       <c r="I30" t="n">
-        <v>0.2367577950734593</v>
+        <v>0.2367578530016597</v>
       </c>
     </row>
     <row r="31">
@@ -3758,7 +3758,7 @@
         <v>0.6613326888173388</v>
       </c>
       <c r="D31" t="n">
-        <v>0.4734979674490238</v>
+        <v>0.4734979102596529</v>
       </c>
       <c r="E31" t="n">
         <v>0.7023809523809523</v>
@@ -3773,7 +3773,7 @@
         <v>0.05295302546837555</v>
       </c>
       <c r="I31" t="n">
-        <v>0.2407877468366905</v>
+        <v>0.2407878040260614</v>
       </c>
     </row>
     <row r="32">
@@ -3787,7 +3787,7 @@
         <v>0.6726636139866308</v>
       </c>
       <c r="D32" t="n">
-        <v>0.4876295123828365</v>
+        <v>0.4876294558034214</v>
       </c>
       <c r="E32" t="n">
         <v>0.7261904761904762</v>
@@ -3802,7 +3802,7 @@
         <v>0.06543162410860737</v>
       </c>
       <c r="I32" t="n">
-        <v>0.2504657257124017</v>
+        <v>0.2504657822918168</v>
       </c>
     </row>
     <row r="33">
@@ -3816,7 +3816,7 @@
         <v>0.6835626973569872</v>
       </c>
       <c r="D33" t="n">
-        <v>0.501405474398645</v>
+        <v>0.5014054184775483</v>
       </c>
       <c r="E33" t="n">
         <v>0.75</v>
@@ -3831,7 +3831,7 @@
         <v>0.0783420645477747</v>
       </c>
       <c r="I33" t="n">
-        <v>0.2604992875061168</v>
+        <v>0.2604993434272136</v>
       </c>
     </row>
     <row r="34">
@@ -3845,7 +3845,7 @@
         <v>0.692234596971832</v>
       </c>
       <c r="D34" t="n">
-        <v>0.5124950288410751</v>
+        <v>0.5124949734944281</v>
       </c>
       <c r="E34" t="n">
         <v>0.7738095238095238</v>
@@ -3860,7 +3860,7 @@
         <v>0.09347968874245371</v>
       </c>
       <c r="I34" t="n">
-        <v>0.2732192568732106</v>
+        <v>0.2732193122198576</v>
       </c>
     </row>
     <row r="35">
@@ -3874,7 +3874,7 @@
         <v>0.7809354664066331</v>
       </c>
       <c r="D35" t="n">
-        <v>0.6326067449452897</v>
+        <v>0.6326066981465766</v>
       </c>
       <c r="E35" t="n">
         <v>0.7976190476190477</v>
@@ -3889,7 +3889,7 @@
         <v>0.0285883431171764</v>
       </c>
       <c r="I35" t="n">
-        <v>0.1769170645785199</v>
+        <v>0.176917111377233</v>
       </c>
     </row>
     <row r="36">
@@ -3903,7 +3903,7 @@
         <v>0.854610684383508</v>
       </c>
       <c r="D36" t="n">
-        <v>0.742198780381028</v>
+        <v>0.7421987446322421</v>
       </c>
       <c r="E36" t="n">
         <v>0.8214285714285714</v>
@@ -3918,7 +3918,7 @@
         <v>0.02127735105017459</v>
       </c>
       <c r="I36" t="n">
-        <v>0.09113455295230533</v>
+        <v>0.09113458870109126</v>
       </c>
     </row>
     <row r="37">
@@ -3926,13 +3926,13 @@
         <v>163.282</v>
       </c>
       <c r="B37" t="n">
-        <v>0.8586272343777037</v>
+        <v>0.8586272343777036</v>
       </c>
       <c r="C37" t="n">
         <v>0.8657650181216239</v>
       </c>
       <c r="D37" t="n">
-        <v>0.7596526993216179</v>
+        <v>0.7596526655848322</v>
       </c>
       <c r="E37" t="n">
         <v>0.8452380952380952</v>
@@ -3941,13 +3941,13 @@
         <v>0.8571428571428571</v>
       </c>
       <c r="G37" t="n">
-        <v>0.001484377234846623</v>
+        <v>0.001484377234846512</v>
       </c>
       <c r="H37" t="n">
         <v>0.00862216097876678</v>
       </c>
       <c r="I37" t="n">
-        <v>0.09749015782123915</v>
+        <v>0.09749019155802485</v>
       </c>
     </row>
     <row r="38">
@@ -3961,7 +3961,7 @@
         <v>0.8916271925727171</v>
       </c>
       <c r="D38" t="n">
-        <v>0.8011010591172846</v>
+        <v>0.8011010304154271</v>
       </c>
       <c r="E38" t="n">
         <v>0.8690476190476191</v>
@@ -3976,7 +3976,7 @@
         <v>0.01067481162033612</v>
       </c>
       <c r="I38" t="n">
-        <v>0.07985132183509636</v>
+        <v>0.0798513505369538</v>
       </c>
     </row>
     <row r="39">
@@ -3987,10 +3987,10 @@
         <v>0.9093774133891683</v>
       </c>
       <c r="C39" t="n">
-        <v>0.9161826338719198</v>
+        <v>0.9161826338719199</v>
       </c>
       <c r="D39" t="n">
-        <v>0.8418607534665039</v>
+        <v>0.8418607300540362</v>
       </c>
       <c r="E39" t="n">
         <v>0.8928571428571429</v>
@@ -4002,10 +4002,10 @@
         <v>0.004615508627263565</v>
       </c>
       <c r="H39" t="n">
-        <v>0.01142072911001502</v>
+        <v>0.01142072911001513</v>
       </c>
       <c r="I39" t="n">
-        <v>0.06290115129540086</v>
+        <v>0.0629011747078686</v>
       </c>
     </row>
     <row r="40">
@@ -4016,10 +4016,10 @@
         <v>0.92143327505439</v>
       </c>
       <c r="C40" t="n">
-        <v>0.9279648136846882</v>
+        <v>0.9279648136846881</v>
       </c>
       <c r="D40" t="n">
-        <v>0.8619755524133155</v>
+        <v>0.8619755317296339</v>
       </c>
       <c r="E40" t="n">
         <v>0.9166666666666666</v>
@@ -4031,10 +4031,10 @@
         <v>0.007138153517038615</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0006066148867404086</v>
+        <v>0.0006066148867405197</v>
       </c>
       <c r="I40" t="n">
-        <v>0.06659587615811313</v>
+        <v>0.06659589684179468</v>
       </c>
     </row>
     <row r="41">
@@ -4045,10 +4045,10 @@
         <v>0.970894911046088</v>
       </c>
       <c r="C41" t="n">
-        <v>0.97495959623665</v>
+        <v>0.9749595962366499</v>
       </c>
       <c r="D41" t="n">
-        <v>0.9471923098832309</v>
+        <v>0.9471923015811593</v>
       </c>
       <c r="E41" t="n">
         <v>0.9404761904761905</v>
@@ -4060,10 +4060,10 @@
         <v>0.01851395866513572</v>
       </c>
       <c r="H41" t="n">
-        <v>0.02257864385569763</v>
+        <v>0.02257864385569752</v>
       </c>
       <c r="I41" t="n">
-        <v>0.005188642497721441</v>
+        <v>0.005188650799793026</v>
       </c>
     </row>
     <row r="42">
@@ -4077,7 +4077,7 @@
         <v>0.9835373561520727</v>
       </c>
       <c r="D42" t="n">
-        <v>0.9640956437008618</v>
+        <v>0.9640956380056943</v>
       </c>
       <c r="E42" t="n">
         <v>0.9642857142857143</v>
@@ -4092,7 +4092,7 @@
         <v>0.007346879961596553</v>
       </c>
       <c r="I42" t="n">
-        <v>0.0120948324896144</v>
+        <v>0.01209483818478185</v>
       </c>
     </row>
     <row r="43">
@@ -4103,10 +4103,10 @@
         <v>0.9847284729833029</v>
       </c>
       <c r="C43" t="n">
-        <v>0.9874179059924982</v>
+        <v>0.9874179059924981</v>
       </c>
       <c r="D43" t="n">
-        <v>0.9719963295893325</v>
+        <v>0.9719963251291137</v>
       </c>
       <c r="E43" t="n">
         <v>0.9880952380952381</v>
@@ -4118,10 +4118,10 @@
         <v>0.0152715270166971</v>
       </c>
       <c r="H43" t="n">
-        <v>0.01258209400750177</v>
+        <v>0.01258209400750188</v>
       </c>
       <c r="I43" t="n">
-        <v>0.02800367041066754</v>
+        <v>0.02800367487088629</v>
       </c>
     </row>
   </sheetData>
@@ -4173,10 +4173,10 @@
         <v>174.3558351446289</v>
       </c>
       <c r="C2" t="n">
-        <v>172.8813583483289</v>
+        <v>172.881358348329</v>
       </c>
       <c r="D2" t="n">
-        <v>195.5984159281983</v>
+        <v>195.5984215432206</v>
       </c>
     </row>
     <row r="3">
@@ -4187,10 +4187,10 @@
         <v>258.5530303380551</v>
       </c>
       <c r="C3" t="n">
-        <v>254.0041188816806</v>
+        <v>254.0041188816808</v>
       </c>
       <c r="D3" t="n">
-        <v>279.2946772672564</v>
+        <v>279.2946828822788</v>
       </c>
     </row>
     <row r="4">
@@ -4201,10 +4201,10 @@
         <v>344.8704606412949</v>
       </c>
       <c r="C4" t="n">
-        <v>336.5174331025025</v>
+        <v>336.5174331025028</v>
       </c>
       <c r="D4" t="n">
-        <v>361.4708714404961</v>
+        <v>361.4708770555184</v>
       </c>
     </row>
     <row r="5">
@@ -4215,10 +4215,10 @@
         <v>437.1556615783541</v>
       </c>
       <c r="C5" t="n">
-        <v>424.1974073653096</v>
+        <v>424.19740736531</v>
       </c>
       <c r="D5" t="n">
-        <v>443.5020779678047</v>
+        <v>443.5020835828271</v>
       </c>
     </row>
     <row r="6">
@@ -4234,7 +4234,7 @@
         <v>774.7162787981323</v>
       </c>
       <c r="D6" t="n">
-        <v>381.8942870284628</v>
+        <v>381.8942269046408</v>
       </c>
     </row>
   </sheetData>
@@ -4289,7 +4289,7 @@
         <v>180.7147711188758</v>
       </c>
       <c r="D2" t="n">
-        <v>212.8178008610142</v>
+        <v>212.8178056693538</v>
       </c>
     </row>
     <row r="3">
@@ -4303,7 +4303,7 @@
         <v>270.3823956259764</v>
       </c>
       <c r="D3" t="n">
-        <v>310.5555680246266</v>
+        <v>310.5555728329663</v>
       </c>
     </row>
     <row r="4">
@@ -4317,7 +4317,7 @@
         <v>363.0073669766706</v>
       </c>
       <c r="D4" t="n">
-        <v>406.5182502758562</v>
+        <v>406.5182550841959</v>
       </c>
     </row>
     <row r="5">
@@ -4331,7 +4331,7 @@
         <v>462.6212541586591</v>
       </c>
       <c r="D5" t="n">
-        <v>502.3116206778718</v>
+        <v>502.3116254862115</v>
       </c>
     </row>
     <row r="6">
@@ -4347,7 +4347,7 @@
         <v>417.2155731215644</v>
       </c>
       <c r="D6" t="n">
-        <v>148.7991547516092</v>
+        <v>148.7991376082626</v>
       </c>
     </row>
   </sheetData>
@@ -4399,10 +4399,10 @@
         <v>176.147146317481</v>
       </c>
       <c r="C2" t="n">
-        <v>173.6438293779424</v>
+        <v>173.6438293779425</v>
       </c>
       <c r="D2" t="n">
-        <v>197.0239888247402</v>
+        <v>197.0239945090367</v>
       </c>
     </row>
     <row r="3">
@@ -4413,10 +4413,10 @@
         <v>258.1170666685379</v>
       </c>
       <c r="C3" t="n">
-        <v>250.7429759414246</v>
+        <v>250.7429759414247</v>
       </c>
       <c r="D3" t="n">
-        <v>279.7002497609799</v>
+        <v>279.7002554452764</v>
       </c>
     </row>
     <row r="4">
@@ -4430,7 +4430,7 @@
         <v>328.0160917679926</v>
       </c>
       <c r="D4" t="n">
-        <v>360.8749684821772</v>
+        <v>360.8749741664736</v>
       </c>
     </row>
     <row r="5">
@@ -4441,10 +4441,10 @@
         <v>429.5454206408473</v>
       </c>
       <c r="C5" t="n">
-        <v>409.1927796756677</v>
+        <v>409.1927796756678</v>
       </c>
       <c r="D5" t="n">
-        <v>441.9064665116047</v>
+        <v>441.9064721959011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plots, sauvegarde et verbose, clean code
</commit_message>
<xml_diff>
--- a/devoir2_results.xlsx
+++ b/devoir2_results.xlsx
@@ -14,6 +14,8 @@
     <sheet name="Return periods Calen 20" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Return periods Calen 25" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Return periods Hydro 20" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Kolmogorov-Smirnov" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Chi-squared" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4176,7 +4178,7 @@
         <v>172.881358348329</v>
       </c>
       <c r="D2" t="n">
-        <v>94.97054954461646</v>
+        <v>175.0626101605569</v>
       </c>
     </row>
     <row r="3">
@@ -4190,7 +4192,7 @@
         <v>254.0041188816808</v>
       </c>
       <c r="D3" t="n">
-        <v>95.03651993429349</v>
+        <v>258.758871499615</v>
       </c>
     </row>
     <row r="4">
@@ -4204,7 +4206,7 @@
         <v>336.5174331025028</v>
       </c>
       <c r="D4" t="n">
-        <v>95.10129218893249</v>
+        <v>340.9350656728547</v>
       </c>
     </row>
     <row r="5">
@@ -4218,7 +4220,7 @@
         <v>424.19740736531</v>
       </c>
       <c r="D5" t="n">
-        <v>95.16595016258273</v>
+        <v>422.9662722001634</v>
       </c>
     </row>
     <row r="6">
@@ -4233,10 +4235,8 @@
       <c r="C6" t="n">
         <v>774.7162787981323</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="D6" t="n">
+        <v>679.3351850034544</v>
       </c>
     </row>
   </sheetData>
@@ -4291,7 +4291,7 @@
         <v>180.7147711188758</v>
       </c>
       <c r="D2" t="n">
-        <v>95.28313411617347</v>
+        <v>188.8317091932907</v>
       </c>
     </row>
     <row r="3">
@@ -4305,7 +4305,7 @@
         <v>270.3823956259764</v>
       </c>
       <c r="D3" t="n">
-        <v>95.33962686340195</v>
+        <v>286.5694763569031</v>
       </c>
     </row>
     <row r="4">
@@ -4319,7 +4319,7 @@
         <v>363.0073669766706</v>
       </c>
       <c r="D4" t="n">
-        <v>95.39509360577912</v>
+        <v>382.5321586081328</v>
       </c>
     </row>
     <row r="5">
@@ -4333,7 +4333,7 @@
         <v>462.6212541586591</v>
       </c>
       <c r="D5" t="n">
-        <v>95.45046248535692</v>
+        <v>478.3255290101483</v>
       </c>
     </row>
     <row r="6">
@@ -4348,10 +4348,8 @@
       <c r="C6" t="n">
         <v>417.2155731215644</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>inf</t>
-        </is>
+      <c r="D6" t="n">
+        <v>264.485804983888</v>
       </c>
     </row>
   </sheetData>
@@ -4406,7 +4404,7 @@
         <v>173.6438293779425</v>
       </c>
       <c r="D2" t="n">
-        <v>97.62441395081817</v>
+        <v>176.7388488797245</v>
       </c>
     </row>
     <row r="3">
@@ -4420,7 +4418,7 @@
         <v>250.7429759414247</v>
       </c>
       <c r="D3" t="n">
-        <v>97.69119823584174</v>
+        <v>259.4151098159642</v>
       </c>
     </row>
     <row r="4">
@@ -4434,7 +4432,7 @@
         <v>328.0160917679926</v>
       </c>
       <c r="D4" t="n">
-        <v>97.7567696040966</v>
+        <v>340.5898285371615</v>
       </c>
     </row>
     <row r="5">
@@ -4448,7 +4446,659 @@
         <v>409.1927796756678</v>
       </c>
       <c r="D5" t="n">
-        <v>97.82222528144584</v>
+        <v>421.6213265665889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Distribution</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>D_max</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>C_alpha</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>alpha</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1084230343935367</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0.1155217666958316</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1088799228167518</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0.09672734580030384</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.09347968874245371</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.09881776540439746</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1882500869537521</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Dataset</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Distribution</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>k_classes</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Chi2_stat</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dof</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Critical_value</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>alpha</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Result</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.539002663778082</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4.46993198906311</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.778731921344894</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5.101257355697612</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.648332938984475</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Calendar 2020</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4.564895208152135</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>4</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.674723409782879</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lognormal: Moments</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7.254192607344461</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Reject H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2.033592561050211</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Lognormal: MaxLikelihood</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7.956985019850496</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Reject H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.76248375215539</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3.841458820694124</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Accept H0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Hydrological 2020</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Gumbel</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>5</v>
+      </c>
+      <c r="D13" t="n">
+        <v>7.388469580311943</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>5.991464547107979</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Reject H0</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>